<commit_message>
add more data in excel
</commit_message>
<xml_diff>
--- a/interview.xlsx
+++ b/interview.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t>Topics</t>
   </si>
@@ -298,9 +298,6 @@
     <t>✓</t>
   </si>
   <si>
-    <t>Notes links</t>
-  </si>
-  <si>
     <t>Videos link</t>
   </si>
   <si>
@@ -377,6 +374,63 @@
   </si>
   <si>
     <t>GFG docker</t>
+  </si>
+  <si>
+    <t>Git oops</t>
+  </si>
+  <si>
+    <t>other Topics</t>
+  </si>
+  <si>
+    <t>AWS lambda</t>
+  </si>
+  <si>
+    <t>Interview question</t>
+  </si>
+  <si>
+    <t>GFG Questions</t>
+  </si>
+  <si>
+    <t>Notes 1</t>
+  </si>
+  <si>
+    <t>Notes 2</t>
+  </si>
+  <si>
+    <t>Question Bank</t>
+  </si>
+  <si>
+    <t>SQL Cheat Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQl query interview </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Design </t>
+  </si>
+  <si>
+    <t>Puzzles gfg</t>
+  </si>
+  <si>
+    <t>Solid principles</t>
+  </si>
+  <si>
+    <t>Solid Principles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFG </t>
+  </si>
+  <si>
+    <t>youtube videos sudocode</t>
+  </si>
+  <si>
+    <t>picture Example</t>
+  </si>
+  <si>
+    <t>Python Code Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git repo </t>
   </si>
 </sst>
 </file>
@@ -435,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -450,9 +504,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -474,11 +525,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,21 +867,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="9" customWidth="1"/>
     <col min="3" max="11" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -835,10 +916,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -850,10 +931,10 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -865,10 +946,10 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -880,10 +961,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -895,10 +976,10 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -910,10 +991,10 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C8" s="2"/>
@@ -927,10 +1008,10 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -942,10 +1023,10 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -957,10 +1038,10 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -972,10 +1053,10 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -987,10 +1068,10 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1002,10 +1083,10 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1017,10 +1098,10 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1032,10 +1113,10 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1047,10 +1128,10 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1062,10 +1143,10 @@
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1077,10 +1158,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1092,221 +1173,308 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A24" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="6" customWidth="1"/>
-    <col min="4" max="6" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="19" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="85.5703125" style="23" customWidth="1"/>
+    <col min="6" max="7" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="D12" s="16"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="24"/>
+    </row>
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="20" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" location="lecture-article"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="D7" r:id="rId4"/>
-    <hyperlink ref="B21" r:id="rId5"/>
-    <hyperlink ref="D11" r:id="rId6"/>
-    <hyperlink ref="D6" r:id="rId7"/>
-    <hyperlink ref="C17" r:id="rId8"/>
-    <hyperlink ref="B15" r:id="rId9"/>
-    <hyperlink ref="B16" r:id="rId10" display="GFG LLD"/>
-    <hyperlink ref="B14" r:id="rId11"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="B22" r:id="rId5"/>
+    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="C18" r:id="rId8"/>
+    <hyperlink ref="B16" r:id="rId9"/>
+    <hyperlink ref="B17" r:id="rId10" display="GFG LLD"/>
+    <hyperlink ref="B15" r:id="rId11"/>
     <hyperlink ref="B3" r:id="rId12"/>
-    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="E3" r:id="rId13"/>
     <hyperlink ref="B2" r:id="rId14"/>
-    <hyperlink ref="D2" r:id="rId15"/>
+    <hyperlink ref="E2" r:id="rId15"/>
     <hyperlink ref="C7" r:id="rId16"/>
     <hyperlink ref="B6" r:id="rId17"/>
+    <hyperlink ref="C15" r:id="rId18"/>
+    <hyperlink ref="B18" r:id="rId19"/>
+    <hyperlink ref="D7" r:id="rId20"/>
+    <hyperlink ref="D3" r:id="rId21"/>
+    <hyperlink ref="C3" r:id="rId22"/>
+    <hyperlink ref="C2" r:id="rId23"/>
+    <hyperlink ref="D6" r:id="rId24"/>
+    <hyperlink ref="D5" r:id="rId25"/>
+    <hyperlink ref="B8" r:id="rId26" display="Puzz;es gfg"/>
+    <hyperlink ref="B14" r:id="rId27"/>
+    <hyperlink ref="E14" r:id="rId28"/>
+    <hyperlink ref="C14" r:id="rId29"/>
+    <hyperlink ref="D14" r:id="rId30"/>
+    <hyperlink ref="B9" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -1315,61 +1483,66 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>106</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="5" t="s">
         <v>100</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>95</v>
+      <c r="B6" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,6 +1757,7 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B3" r:id="rId4"/>
     <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>